<commit_message>
all pages are finished
</commit_message>
<xml_diff>
--- a/Excels/ABA Customer Info.xlsx
+++ b/Excels/ABA Customer Info.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brock.ullyott\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tszyeunglam/GitHub/CPSC471_Project/Excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="4780" yWindow="3040" windowWidth="25980" windowHeight="9040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
   <si>
     <t>Age</t>
   </si>
@@ -41,9 +47,6 @@
     <t>First Name</t>
   </si>
   <si>
-    <t>Reservation Number</t>
-  </si>
-  <si>
     <t>Alana</t>
   </si>
   <si>
@@ -93,16 +96,90 @@
   </si>
   <si>
     <t>Andrews</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>England</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>alana@nomail.com</t>
+  </si>
+  <si>
+    <t>archie@nomail.com</t>
+  </si>
+  <si>
+    <t>betty@nomail.com</t>
+  </si>
+  <si>
+    <t>veronica@nomail.com</t>
+  </si>
+  <si>
+    <t>brianna@nomail.com</t>
+  </si>
+  <si>
+    <t>chrissy@nomail.com</t>
+  </si>
+  <si>
+    <t>derrick@nomail.com</t>
+  </si>
+  <si>
+    <t>cooper@nomail.com</t>
+  </si>
+  <si>
+    <t>alan@nomail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -125,13 +202,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -410,22 +490,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="33.1640625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="34.85546875" customWidth="1"/>
-    <col min="6" max="6" width="37.85546875" customWidth="1"/>
+    <col min="4" max="4" width="34.83203125" customWidth="1"/>
+    <col min="6" max="6" width="37.83203125" customWidth="1"/>
+    <col min="8" max="8" width="18.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -442,190 +524,289 @@
         <v>0</v>
       </c>
       <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
       <c r="C2">
         <v>123456</v>
       </c>
       <c r="D2">
-        <v>111111111</v>
+        <v>123456789</v>
       </c>
       <c r="E2">
         <v>25</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2">
+        <v>3214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
       </c>
       <c r="C3">
         <v>987654</v>
       </c>
       <c r="D3">
-        <v>123456789</v>
+        <v>133456789</v>
       </c>
       <c r="E3">
         <v>32</v>
       </c>
-      <c r="F3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
       </c>
       <c r="C4">
         <v>587534</v>
       </c>
       <c r="D4">
-        <v>545645789</v>
+        <v>986754382</v>
       </c>
       <c r="E4">
-        <v>28</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4">
+        <v>5454</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
       </c>
       <c r="C5">
         <v>578742</v>
       </c>
       <c r="D5">
-        <v>455855211</v>
+        <v>364527183</v>
       </c>
       <c r="E5">
         <v>28</v>
       </c>
-      <c r="F5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5">
+        <v>6565</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
       </c>
       <c r="C6">
         <v>751235</v>
       </c>
       <c r="D6">
-        <v>187321456</v>
+        <v>321321312</v>
       </c>
       <c r="E6">
-        <v>25</v>
-      </c>
-      <c r="F6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6">
+        <v>7676</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
       </c>
       <c r="C7">
         <v>782100</v>
       </c>
       <c r="D7">
-        <v>648124862</v>
+        <v>654654654</v>
       </c>
       <c r="E7">
         <v>26</v>
       </c>
-      <c r="F7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7">
+        <v>4344</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
         <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>19</v>
       </c>
       <c r="C8">
         <v>985522</v>
       </c>
       <c r="D8">
-        <v>674125836</v>
+        <v>888999000</v>
       </c>
       <c r="E8">
-        <v>29</v>
-      </c>
-      <c r="F8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8">
+        <v>9796</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9">
         <v>336655</v>
       </c>
       <c r="D9">
-        <v>110220330</v>
+        <v>970960593</v>
       </c>
       <c r="E9">
         <v>29</v>
       </c>
-      <c r="F9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9">
+        <v>6043</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
       </c>
       <c r="C10">
         <v>665522</v>
       </c>
       <c r="D10">
-        <v>446655881</v>
+        <v>563018920</v>
       </c>
       <c r="E10">
         <v>39</v>
       </c>
-      <c r="F10">
-        <v>9</v>
+      <c r="F10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I10">
+        <v>2389</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H9" r:id="rId2"/>
+    <hyperlink ref="H8" r:id="rId3"/>
+    <hyperlink ref="H7" r:id="rId4"/>
+    <hyperlink ref="H6" r:id="rId5"/>
+    <hyperlink ref="H5" r:id="rId6"/>
+    <hyperlink ref="H4" r:id="rId7"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated all pages and some CSV
</commit_message>
<xml_diff>
--- a/Excels/ABA Customer Info.xlsx
+++ b/Excels/ABA Customer Info.xlsx
@@ -134,9 +134,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
     <t>alana@nomail.com</t>
   </si>
   <si>
@@ -162,6 +159,9 @@
   </si>
   <si>
     <t>alan@nomail.com</t>
+  </si>
+  <si>
+    <t>Username</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -530,7 +530,7 @@
         <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="I1" t="s">
         <v>33</v>
@@ -559,7 +559,7 @@
         <v>31</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I2">
         <v>3214</v>
@@ -588,7 +588,7 @@
         <v>32</v>
       </c>
       <c r="H3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I3">
         <v>3232</v>
@@ -617,7 +617,7 @@
         <v>32</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I4">
         <v>5454</v>
@@ -646,7 +646,7 @@
         <v>32</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I5">
         <v>6565</v>
@@ -675,7 +675,7 @@
         <v>31</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I6">
         <v>7676</v>
@@ -704,7 +704,7 @@
         <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I7">
         <v>4344</v>
@@ -733,7 +733,7 @@
         <v>31</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I8">
         <v>9796</v>
@@ -762,7 +762,7 @@
         <v>31</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I9">
         <v>6043</v>
@@ -791,7 +791,7 @@
         <v>32</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I10">
         <v>2389</v>

</xml_diff>